<commit_message>
testes on flux implementation, litle success
</commit_message>
<xml_diff>
--- a/methanolA_HIFIdata_k0.xlsx
+++ b/methanolA_HIFIdata_k0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcaprod_ucl_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcaprod_ucl_ac_uk/Documents/Desktop/UCL/Year3/group project/codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F57C0AF-086E-4CA8-AF3C-3189A5F2D5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8F57C0AF-086E-4CA8-AF3C-3189A5F2D5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F511DC7D-7428-4F1C-B9F6-B40BE839699E}"/>
   <bookViews>
-    <workbookView xWindow="26190" yWindow="5475" windowWidth="21420" windowHeight="12825" xr2:uid="{71A87D2A-6272-484F-8BF5-F1944B0D0F69}"/>
+    <workbookView xWindow="0" yWindow="2880" windowWidth="43665" windowHeight="12825" xr2:uid="{71A87D2A-6272-484F-8BF5-F1944B0D0F69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -550,6 +550,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="72" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>